<commit_message>
header set value is ok
</commit_message>
<xml_diff>
--- a/case/c2/c2.xlsx
+++ b/case/c2/c2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="5320" yWindow="0" windowWidth="20280" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="apis" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assert_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://api-promotion.test.rs.com/subPromotion/skuList</t>
   </si>
   <si>
@@ -76,18 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>import requests
-params = {"mobilePhone" : "18217629954",
-              "password" : "wap123456"
-    }
-   getRsponse("http://longguo.dev.rs.com/api/userInfoV2/login" ,
-                        params,
-                        "json",
-                        {}
-                        )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>api_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -131,10 +115,6 @@
   </si>
   <si>
     <t>header_3_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>assert_3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -165,6 +145,71 @@
   </si>
   <si>
     <t>E/B端费用单列表查询</t>
+  </si>
+  <si>
+    <t>api_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>import requests
+params = {"mobilePhone" : "18217629954",
+              "password" : "wap123456"
+    }
+   getRsponse("http://longguo.dev.rs.com/api/userInfoV2/login" ,
+                        params,
+                        "json",
+                        {}
+                        )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>param_1_json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"mobilePhone" : "18217629954",
+              "password" : "wap123456"
+    }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assert_1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assert_2_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assert_3_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header_2_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resCode</t>
+  </si>
+  <si>
+    <t>$api_1_response_data$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header_3_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -223,7 +268,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,6 +293,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -257,7 +310,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="23"/>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="32">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -281,6 +334,14 @@
     <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -626,43 +687,57 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>30</v>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -676,25 +751,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="68.5" customWidth="1"/>
-    <col min="3" max="3" width="57.1640625" customWidth="1"/>
+    <col min="3" max="3" width="57.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="356" customHeight="1">
+    <row r="1" spans="1:2" ht="45">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="356" customHeight="1">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -711,10 +794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -725,28 +808,39 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -766,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -779,24 +873,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -813,10 +907,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -827,18 +921,41 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20" customHeight="1">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -863,39 +980,40 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>18217629954</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="135">
       <c r="A30" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>